<commit_message>
updates to our checklist
</commit_message>
<xml_diff>
--- a/project3_req_checklist.xlsx
+++ b/project3_req_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin Tran\project_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47166668-9199-4EC0-B83E-315C35FB9037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8E470B-D0B0-475B-94EB-44DE808F876C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{7DAC2924-F08F-4315-8F85-E31847044D06}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Project 3 Requirements Checklist </t>
   </si>
@@ -96,7 +96,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Google Charts ?</t>
+    <t>To be fulfilled by Thursday September 30th 2021</t>
+  </si>
+  <si>
+    <t>FullChart</t>
   </si>
 </sst>
 </file>
@@ -574,14 +577,16 @@
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>